<commit_message>
comparing fim with and without stimulus
</commit_message>
<xml_diff>
--- a/reports/dec-fim.xlsx
+++ b/reports/dec-fim.xlsx
@@ -679,7 +679,7 @@
         <v>0.03946169552298145</v>
       </c>
       <c r="C2">
-        <v>-0.0811218478370582</v>
+        <v>-0.08112184783705709</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -799,7 +799,7 @@
         <v>0</v>
       </c>
       <c r="AQ2">
-        <v>1389.136</v>
+        <v>1388.7</v>
       </c>
       <c r="AR2">
         <v>1650.8</v>
@@ -826,7 +826,7 @@
         <v>192.814</v>
       </c>
       <c r="AZ2">
-        <v>739.664</v>
+        <v>740.0999999999999</v>
       </c>
       <c r="BA2">
         <v>29.8</v>
@@ -835,7 +835,7 @@
         <v>0</v>
       </c>
       <c r="BC2">
-        <v>163.864</v>
+        <v>164.3</v>
       </c>
       <c r="BD2">
         <v>477</v>
@@ -861,10 +861,10 @@
         <v>43190</v>
       </c>
       <c r="B3">
-        <v>0.01842065120159704</v>
+        <v>0.01842065120159805</v>
       </c>
       <c r="C3">
-        <v>-0.02387626252182858</v>
+        <v>-0.0238762625218272</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -984,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="AQ3">
-        <v>1428.501</v>
+        <v>1428.1</v>
       </c>
       <c r="AR3">
         <v>1598.6</v>
@@ -1011,7 +1011,7 @@
         <v>192.605</v>
       </c>
       <c r="AZ3">
-        <v>746.299</v>
+        <v>746.7</v>
       </c>
       <c r="BA3">
         <v>29.2</v>
@@ -1020,7 +1020,7 @@
         <v>0</v>
       </c>
       <c r="BC3">
-        <v>164.499</v>
+        <v>164.9</v>
       </c>
       <c r="BD3">
         <v>487</v>
@@ -1046,10 +1046,10 @@
         <v>43281</v>
       </c>
       <c r="B4">
-        <v>0.4273326313133025</v>
+        <v>0.4273326313133015</v>
       </c>
       <c r="C4">
-        <v>0.06409033606477539</v>
+        <v>0.06409033606477599</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>1431.708</v>
+        <v>1431.3</v>
       </c>
       <c r="AR4">
         <v>1608.9</v>
@@ -1196,7 +1196,7 @@
         <v>205.743</v>
       </c>
       <c r="AZ4">
-        <v>756.7919999999999</v>
+        <v>757.1999999999999</v>
       </c>
       <c r="BA4">
         <v>27.9</v>
@@ -1205,7 +1205,7 @@
         <v>0</v>
       </c>
       <c r="BC4">
-        <v>164.192</v>
+        <v>164.5999999999999</v>
       </c>
       <c r="BD4">
         <v>455.5</v>
@@ -1231,10 +1231,10 @@
         <v>43373</v>
       </c>
       <c r="B5">
-        <v>0.1652983376755857</v>
+        <v>0.1652983376755887</v>
       </c>
       <c r="C5">
-        <v>0.1626283289283671</v>
+        <v>0.162628328928369</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1354,7 +1354,7 @@
         <v>0</v>
       </c>
       <c r="AQ5">
-        <v>1435.211</v>
+        <v>1434.8</v>
       </c>
       <c r="AR5">
         <v>1628.3</v>
@@ -1381,7 +1381,7 @@
         <v>202.584</v>
       </c>
       <c r="AZ5">
-        <v>760.289</v>
+        <v>760.6999999999999</v>
       </c>
       <c r="BA5">
         <v>27.4</v>
@@ -1390,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="BC5">
-        <v>165.1889999999999</v>
+        <v>165.6</v>
       </c>
       <c r="BD5">
         <v>472.2</v>
@@ -1416,10 +1416,10 @@
         <v>43465</v>
       </c>
       <c r="B6">
-        <v>-0.4280824757189858</v>
+        <v>-0.4280824757189849</v>
       </c>
       <c r="C6">
-        <v>0.04574228611787533</v>
+        <v>0.04574228611787742</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1539,7 +1539,7 @@
         <v>0</v>
       </c>
       <c r="AQ6">
-        <v>1440.553</v>
+        <v>1440.2</v>
       </c>
       <c r="AR6">
         <v>1634.2</v>
@@ -1566,7 +1566,7 @@
         <v>200.1759999999999</v>
       </c>
       <c r="AZ6">
-        <v>755.447</v>
+        <v>755.8</v>
       </c>
       <c r="BA6">
         <v>27</v>
@@ -1575,7 +1575,7 @@
         <v>0</v>
       </c>
       <c r="BC6">
-        <v>165.647</v>
+        <v>166</v>
       </c>
       <c r="BD6">
         <v>456.5</v>
@@ -1601,10 +1601,10 @@
         <v>43555</v>
       </c>
       <c r="B7">
-        <v>0.211407231042728</v>
+        <v>0.211407231042727</v>
       </c>
       <c r="C7">
-        <v>0.09398893107815808</v>
+        <v>0.09398893107815967</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1724,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="AQ7">
-        <v>1503.843</v>
+        <v>1503.4</v>
       </c>
       <c r="AR7">
         <v>1695.5</v>
@@ -1751,7 +1751,7 @@
         <v>194.871</v>
       </c>
       <c r="AZ7">
-        <v>766.2570000000001</v>
+        <v>766.7</v>
       </c>
       <c r="BA7">
         <v>28</v>
@@ -1760,7 +1760,7 @@
         <v>0</v>
       </c>
       <c r="BC7">
-        <v>166.8570000000001</v>
+        <v>167.3000000000001</v>
       </c>
       <c r="BD7">
         <v>475.2</v>
@@ -1786,10 +1786,10 @@
         <v>43646</v>
       </c>
       <c r="B8">
-        <v>0.6139640220240625</v>
+        <v>0.6139640220240616</v>
       </c>
       <c r="C8">
-        <v>0.1406467787558481</v>
+        <v>0.1406467787558497</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1909,7 +1909,7 @@
         <v>0</v>
       </c>
       <c r="AQ8">
-        <v>1509.005</v>
+        <v>1508.6</v>
       </c>
       <c r="AR8">
         <v>1703.1</v>
@@ -1936,7 +1936,7 @@
         <v>195.328</v>
       </c>
       <c r="AZ8">
-        <v>782.2950000000001</v>
+        <v>782.7</v>
       </c>
       <c r="BA8">
         <v>27.5</v>
@@ -1945,7 +1945,7 @@
         <v>0</v>
       </c>
       <c r="BC8">
-        <v>167.2950000000001</v>
+        <v>167.7</v>
       </c>
       <c r="BD8">
         <v>519.4</v>
@@ -1971,10 +1971,10 @@
         <v>43738</v>
       </c>
       <c r="B9">
-        <v>0.4001201119220791</v>
+        <v>0.4001201119220801</v>
       </c>
       <c r="C9">
-        <v>0.1993522223174715</v>
+        <v>0.1993522223174726</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -2094,7 +2094,7 @@
         <v>0</v>
       </c>
       <c r="AQ9">
-        <v>1514.303</v>
+        <v>1513.9</v>
       </c>
       <c r="AR9">
         <v>1713.2</v>
@@ -2121,7 +2121,7 @@
         <v>203.4759999999999</v>
       </c>
       <c r="AZ9">
-        <v>790.597</v>
+        <v>791</v>
       </c>
       <c r="BA9">
         <v>27.6</v>
@@ -2130,7 +2130,7 @@
         <v>0</v>
       </c>
       <c r="BC9">
-        <v>168.2970000000001</v>
+        <v>168.7000000000001</v>
       </c>
       <c r="BD9">
         <v>483.9</v>
@@ -2156,10 +2156,10 @@
         <v>43830</v>
       </c>
       <c r="B10">
-        <v>0.4816080942708365</v>
+        <v>0.4816080942708375</v>
       </c>
       <c r="C10">
-        <v>0.426774864814927</v>
+        <v>0.4267748648149282</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -2279,7 +2279,7 @@
         <v>0</v>
       </c>
       <c r="AQ10">
-        <v>1522.308</v>
+        <v>1521.9</v>
       </c>
       <c r="AR10">
         <v>1740.2</v>
@@ -2306,7 +2306,7 @@
         <v>207.991</v>
       </c>
       <c r="AZ10">
-        <v>788.492</v>
+        <v>788.9</v>
       </c>
       <c r="BA10">
         <v>27.9</v>
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="BC10">
-        <v>169.092</v>
+        <v>169.5</v>
       </c>
       <c r="BD10">
         <v>480.9</v>
@@ -2341,10 +2341,10 @@
         <v>43921</v>
       </c>
       <c r="B11">
-        <v>0.08506766165855074</v>
+        <v>0.08506766165855166</v>
       </c>
       <c r="C11">
-        <v>0.3951899724688828</v>
+        <v>0.3951899724688844</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2464,7 +2464,7 @@
         <v>0</v>
       </c>
       <c r="AQ11">
-        <v>1574.779</v>
+        <v>1574.4</v>
       </c>
       <c r="AR11">
         <v>1756.6</v>
@@ -2491,7 +2491,7 @@
         <v>200.671</v>
       </c>
       <c r="AZ11">
-        <v>810.121</v>
+        <v>810.5</v>
       </c>
       <c r="BA11">
         <v>43.4</v>
@@ -2500,7 +2500,7 @@
         <v>0</v>
       </c>
       <c r="BC11">
-        <v>186.021</v>
+        <v>186.4</v>
       </c>
       <c r="BD11">
         <v>495.8</v>
@@ -2526,10 +2526,10 @@
         <v>44012</v>
       </c>
       <c r="B12">
-        <v>14.28977758476562</v>
+        <v>14.28977758476561</v>
       </c>
       <c r="C12">
-        <v>3.814143363154271</v>
+        <v>3.814143363154272</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2613,7 +2613,7 @@
         <v>5627.4</v>
       </c>
       <c r="AE12">
-        <v>4134.600000000001</v>
+        <v>4134.6</v>
       </c>
       <c r="AF12">
         <v>2096.5</v>
@@ -2649,7 +2649,7 @@
         <v>1078.1</v>
       </c>
       <c r="AQ12">
-        <v>3763.789333333334</v>
+        <v>3741.533333333334</v>
       </c>
       <c r="AR12">
         <v>1600.1</v>
@@ -2676,16 +2676,16 @@
         <v>156.16</v>
       </c>
       <c r="AZ12">
-        <v>1039.610666666667</v>
+        <v>1061.866666666667</v>
       </c>
       <c r="BA12">
-        <v>277.6</v>
+        <v>249.0666666666667</v>
       </c>
       <c r="BB12">
         <v>0</v>
       </c>
       <c r="BC12">
-        <v>370.810666666667</v>
+        <v>393.0666666666668</v>
       </c>
       <c r="BD12">
         <v>496.4</v>
@@ -2711,10 +2711,10 @@
         <v>44104</v>
       </c>
       <c r="B13">
-        <v>3.607238917645105</v>
+        <v>3.607238917645103</v>
       </c>
       <c r="C13">
-        <v>4.615923064585028</v>
+        <v>4.615923064585027</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2828,13 +2828,13 @@
         <v>1328.772</v>
       </c>
       <c r="AO13">
-        <v>738.2</v>
+        <v>695.2</v>
       </c>
       <c r="AP13">
         <v>15.6</v>
       </c>
       <c r="AQ13">
-        <v>2653.267</v>
+        <v>2615.2</v>
       </c>
       <c r="AR13">
         <v>1687.4</v>
@@ -2861,16 +2861,16 @@
         <v>197.628</v>
       </c>
       <c r="AZ13">
-        <v>827.433</v>
+        <v>865.5</v>
       </c>
       <c r="BA13">
-        <v>140</v>
+        <v>186</v>
       </c>
       <c r="BB13">
         <v>0</v>
       </c>
       <c r="BC13">
-        <v>143.7329999999999</v>
+        <v>181.8</v>
       </c>
       <c r="BD13">
         <v>506.6</v>
@@ -2896,10 +2896,10 @@
         <v>44196</v>
       </c>
       <c r="B14">
-        <v>-3.101195725775879</v>
+        <v>-2.144250383721548</v>
       </c>
       <c r="C14">
-        <v>3.720222109573349</v>
+        <v>3.95945844508693</v>
       </c>
       <c r="E14">
         <v>21598.39917290762</v>
@@ -2932,7 +2932,7 @@
         <v>504.62142385961</v>
       </c>
       <c r="O14">
-        <v>298.3728847770673</v>
+        <v>298.4243775484318</v>
       </c>
       <c r="P14">
         <v>74.40802956971426</v>
@@ -2974,13 +2974,13 @@
         <v>1552.349397498257</v>
       </c>
       <c r="AC14">
-        <v>337.8</v>
+        <v>874.878</v>
       </c>
       <c r="AD14">
-        <v>3977.346150498898</v>
+        <v>3981.231964941214</v>
       </c>
       <c r="AE14">
-        <v>2189.849621653418</v>
+        <v>2200.735436095733</v>
       </c>
       <c r="AF14">
         <v>2211.584932832352</v>
@@ -2992,10 +2992,10 @@
         <v>1518.488074228699</v>
       </c>
       <c r="AI14">
-        <v>5204.843295004225</v>
+        <v>5205.9886129062</v>
       </c>
       <c r="AJ14">
-        <v>309.1843422640096</v>
+        <v>309.2395471855706</v>
       </c>
       <c r="AK14">
         <v>383.5339732930983</v>
@@ -3010,13 +3010,13 @@
         <v>1368.117371850785</v>
       </c>
       <c r="AO14">
-        <v>257.8</v>
+        <v>738.2</v>
       </c>
       <c r="AP14">
         <v>0</v>
       </c>
       <c r="AQ14">
-        <v>1966.882334153418</v>
+        <v>1932.605981095733</v>
       </c>
       <c r="AR14">
         <v>1694.740626374956</v>
@@ -3043,16 +3043,16 @@
         <v>184.2320256474721</v>
       </c>
       <c r="AZ14">
-        <v>829.5015824999999</v>
+        <v>867.6637499999999</v>
       </c>
       <c r="BA14">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="BB14">
         <v>0</v>
       </c>
       <c r="BC14">
-        <v>222.9672875</v>
+        <v>268.129455</v>
       </c>
       <c r="BD14">
         <v>516.8443064573955</v>
@@ -3064,10 +3064,10 @@
         <v>1371.688057702267</v>
       </c>
       <c r="BG14">
-        <v>1908.045515190684</v>
+        <v>1909.190833092659</v>
       </c>
       <c r="BH14">
-        <v>91.96879121435907</v>
+        <v>92.02399613592002</v>
       </c>
       <c r="BI14">
         <v>0.6019649465167092</v>
@@ -3078,10 +3078,10 @@
         <v>44286</v>
       </c>
       <c r="B15">
-        <v>3.932030374331585</v>
+        <v>3.383617228811452</v>
       </c>
       <c r="C15">
-        <v>4.681962787741607</v>
+        <v>4.784095836875155</v>
       </c>
       <c r="E15">
         <v>21956.60675467075</v>
@@ -3102,7 +3102,7 @@
         <v>0.002172328543681434</v>
       </c>
       <c r="K15">
-        <v>1575.75145528078</v>
+        <v>1504.35145528078</v>
       </c>
       <c r="L15">
         <v>736.6971955181332</v>
@@ -3114,7 +3114,7 @@
         <v>523.17084771922</v>
       </c>
       <c r="O15">
-        <v>341.1409954476429</v>
+        <v>341.1926948948232</v>
       </c>
       <c r="P15">
         <v>74.70668003712791</v>
@@ -3123,7 +3123,7 @@
         <v>0.003938982612060604</v>
       </c>
       <c r="R15">
-        <v>2400.26256</v>
+        <v>2341.26256</v>
       </c>
       <c r="S15">
         <v>0.0031885362715387</v>
@@ -3153,16 +3153,16 @@
         <v>735.8825618131279</v>
       </c>
       <c r="AB15">
-        <v>1573.922904250773</v>
+        <v>1585.922904250773</v>
       </c>
       <c r="AC15">
-        <v>724</v>
+        <v>-6.476</v>
       </c>
       <c r="AD15">
-        <v>3702.613611385422</v>
+        <v>3709.608928678839</v>
       </c>
       <c r="AE15">
-        <v>2628.550212573491</v>
+        <v>3299.545529866908</v>
       </c>
       <c r="AF15">
         <v>2227.497377316697</v>
@@ -3174,31 +3174,31 @@
         <v>1543.33741852472</v>
       </c>
       <c r="AI15">
-        <v>5265.785844618473</v>
+        <v>5266.950157518768</v>
       </c>
       <c r="AJ15">
-        <v>320.9251877595512</v>
+        <v>320.9813082499604</v>
       </c>
       <c r="AK15">
         <v>578.0209212961762</v>
       </c>
       <c r="AL15">
-        <v>0</v>
+        <v>664</v>
       </c>
       <c r="AM15">
         <v>523.17084771922</v>
       </c>
       <c r="AN15">
-        <v>1387.852444352445</v>
+        <v>1399.852444352445</v>
       </c>
       <c r="AO15">
-        <v>664</v>
+        <v>43</v>
       </c>
       <c r="AP15">
         <v>664</v>
       </c>
       <c r="AQ15">
-        <v>2425.225506854741</v>
+        <v>3057.963251229407</v>
       </c>
       <c r="AR15">
         <v>1702.081252749912</v>
@@ -3225,16 +3225,16 @@
         <v>186.0704598983283</v>
       </c>
       <c r="AZ15">
-        <v>831.5753364562498</v>
+        <v>869.8329093749999</v>
       </c>
       <c r="BA15">
-        <v>60</v>
+        <v>-46</v>
       </c>
       <c r="BB15">
         <v>0</v>
       </c>
       <c r="BC15">
-        <v>203.32470571875</v>
+        <v>241.5822786375001</v>
       </c>
       <c r="BD15">
         <v>525.4161245667848</v>
@@ -3246,10 +3246,10 @@
         <v>1394.437385471856</v>
       </c>
       <c r="BG15">
-        <v>1939.690284991389</v>
+        <v>1940.854597891685</v>
       </c>
       <c r="BH15">
-        <v>93.49408566025009</v>
+        <v>93.55020615065929</v>
       </c>
       <c r="BI15">
         <v>0.6040046295094899</v>
@@ -3260,10 +3260,10 @@
         <v>44377</v>
       </c>
       <c r="B16">
-        <v>-2.069715247260751</v>
+        <v>-5.508113222542727</v>
       </c>
       <c r="C16">
-        <v>0.5920895797350152</v>
+        <v>-0.1653768649519298</v>
       </c>
       <c r="E16">
         <v>22305.74845884954</v>
@@ -3284,7 +3284,7 @@
         <v>0.003434875674763305</v>
       </c>
       <c r="K16">
-        <v>1582.652602267454</v>
+        <v>1511.252602267454</v>
       </c>
       <c r="L16">
         <v>740.0767619173906</v>
@@ -3296,7 +3296,7 @@
         <v>541.72027157883</v>
       </c>
       <c r="O16">
-        <v>314.0224339220724</v>
+        <v>314.074370538223</v>
       </c>
       <c r="P16">
         <v>75.04939368825832</v>
@@ -3305,7 +3305,7 @@
         <v>0.00541033706720695</v>
       </c>
       <c r="R16">
-        <v>2406.1157164</v>
+        <v>2347.1157164</v>
       </c>
       <c r="S16">
         <v>0.005802914123625325</v>
@@ -3335,16 +3335,16 @@
         <v>761.973842719692</v>
       </c>
       <c r="AB16">
-        <v>1589.729869596065</v>
+        <v>1613.876822716431</v>
       </c>
       <c r="AC16">
-        <v>152</v>
+        <v>344.8</v>
       </c>
       <c r="AD16">
-        <v>3479.229843411781</v>
+        <v>3488.775830340336</v>
       </c>
       <c r="AE16">
-        <v>2044.1945694545</v>
+        <v>2053.740556383055</v>
       </c>
       <c r="AF16">
         <v>2243.192877611105</v>
@@ -3356,10 +3356,10 @@
         <v>1567.610999963712</v>
       </c>
       <c r="AI16">
-        <v>5325.927496586201</v>
+        <v>5327.110323740309</v>
       </c>
       <c r="AJ16">
-        <v>332.6274295698818</v>
+        <v>332.6844424570025</v>
       </c>
       <c r="AK16">
         <v>578.0231042240816</v>
@@ -3371,16 +3371,16 @@
         <v>541.72027157883</v>
       </c>
       <c r="AN16">
-        <v>1403.659409697737</v>
+        <v>1427.806362818103</v>
       </c>
       <c r="AO16">
-        <v>108</v>
+        <v>257.8</v>
       </c>
       <c r="AP16">
         <v>0</v>
       </c>
       <c r="AQ16">
-        <v>1856.511551971453</v>
+        <v>1827.704322048961</v>
       </c>
       <c r="AR16">
         <v>1709.421879124869</v>
@@ -3407,16 +3407,16 @@
         <v>186.0704598983282</v>
       </c>
       <c r="AZ16">
-        <v>833.6542747973904</v>
+        <v>872.0074916484373</v>
       </c>
       <c r="BA16">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="BB16">
         <v>0</v>
       </c>
       <c r="BC16">
-        <v>187.6830174830469</v>
+        <v>226.0362343340938</v>
       </c>
       <c r="BD16">
         <v>533.7709984862367</v>
@@ -3428,10 +3428,10 @@
         <v>1416.610950384416</v>
       </c>
       <c r="BG16">
-        <v>1970.534157145576</v>
+        <v>1971.716984299685</v>
       </c>
       <c r="BH16">
-        <v>94.98077642093004</v>
+        <v>95.03778930805085</v>
       </c>
       <c r="BI16">
         <v>0.6061875574147406</v>
@@ -3442,10 +3442,10 @@
         <v>44469</v>
       </c>
       <c r="B17">
-        <v>-4.698336107940325</v>
+        <v>2.048668124438896</v>
       </c>
       <c r="C17">
-        <v>-1.484304176661342</v>
+        <v>-0.5550195632534816</v>
       </c>
       <c r="E17">
         <v>22678.92528034497</v>
@@ -3466,7 +3466,7 @@
         <v>0.003821926349092397</v>
       </c>
       <c r="K17">
-        <v>1549.936803023271</v>
+        <v>1590.736803023271</v>
       </c>
       <c r="L17">
         <v>744.0356825565207</v>
@@ -3478,7 +3478,7 @@
         <v>560.2696954384398</v>
       </c>
       <c r="O17">
-        <v>315.0549761349776</v>
+        <v>315.107190577634</v>
       </c>
       <c r="P17">
         <v>75.45085825101107</v>
@@ -3517,16 +3517,16 @@
         <v>788.0651236262559</v>
       </c>
       <c r="AB17">
-        <v>1600.433864524897</v>
+        <v>1636.87652348763</v>
       </c>
       <c r="AC17">
-        <v>44</v>
+        <v>724</v>
       </c>
       <c r="AD17">
-        <v>3322.170295467558</v>
+        <v>3333.663631241299</v>
       </c>
       <c r="AE17">
-        <v>1856.66914790213</v>
+        <v>1868.162483675872</v>
       </c>
       <c r="AF17">
         <v>2259.463532269534</v>
@@ -3538,10 +3538,10 @@
         <v>1593.411022465526</v>
       </c>
       <c r="AI17">
-        <v>5388.192458593532</v>
+        <v>5389.395074533414</v>
       </c>
       <c r="AJ17">
-        <v>344.4320160340274</v>
+        <v>344.4899827509665</v>
       </c>
       <c r="AK17">
         <v>578.0254615370975</v>
@@ -3553,7 +3553,7 @@
         <v>560.2696954384398</v>
       </c>
       <c r="AN17">
-        <v>1414.363404626569</v>
+        <v>1450.806063589301</v>
       </c>
       <c r="AO17">
         <v>0</v>
@@ -3562,7 +3562,7 @@
         <v>0</v>
       </c>
       <c r="AQ17">
-        <v>1668.267715331668</v>
+        <v>1641.216068170108</v>
       </c>
       <c r="AR17">
         <v>1716.762505499825</v>
@@ -3589,16 +3589,16 @@
         <v>186.0704598983283</v>
       </c>
       <c r="AZ17">
-        <v>837.8225461713772</v>
+        <v>876.3675291066794</v>
       </c>
       <c r="BA17">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="BB17">
         <v>0</v>
       </c>
       <c r="BC17">
-        <v>188.4014325704621</v>
+        <v>226.9464155057643</v>
       </c>
       <c r="BD17">
         <v>542.7010267697088</v>
@@ -3610,10 +3610,10 @@
         <v>1440.310956359798</v>
       </c>
       <c r="BG17">
-        <v>2003.501339339367</v>
+        <v>2004.703955279249</v>
       </c>
       <c r="BH17">
-        <v>96.56981183542507</v>
+        <v>96.62777855236428</v>
       </c>
       <c r="BI17">
         <v>0.6085448704308245</v>
@@ -3624,10 +3624,10 @@
         <v>44561</v>
       </c>
       <c r="B18">
-        <v>-2.286601610844267</v>
+        <v>-1.058292142645675</v>
       </c>
       <c r="C18">
-        <v>-1.280655647928439</v>
+        <v>-0.2835300029845134</v>
       </c>
       <c r="E18">
         <v>22928.86941700194</v>
@@ -3648,7 +3648,7 @@
         <v>0.003422428967105207</v>
       </c>
       <c r="K18">
-        <v>1561.597960524671</v>
+        <v>1602.397960524671</v>
       </c>
       <c r="L18">
         <v>749.7462776422768</v>
@@ -3660,7 +3660,7 @@
         <v>554.6929574085671</v>
       </c>
       <c r="O18">
-        <v>310.5443796932509</v>
+        <v>310.5969948902631</v>
       </c>
       <c r="P18">
         <v>76.02995588093096</v>
@@ -3699,16 +3699,16 @@
         <v>780.2209857392268</v>
       </c>
       <c r="AB18">
-        <v>1636.414640755323</v>
+        <v>1673.784384760761</v>
       </c>
       <c r="AC18">
-        <v>44</v>
+        <v>152</v>
       </c>
       <c r="AD18">
-        <v>3414.460892969204</v>
+        <v>3425.306801055291</v>
       </c>
       <c r="AE18">
-        <v>1854.056174376382</v>
+        <v>1864.902082462469</v>
       </c>
       <c r="AF18">
         <v>2286.970123544343</v>
@@ -3720,10 +3720,10 @@
         <v>1613.043268745998</v>
       </c>
       <c r="AI18">
-        <v>5458.840776079058</v>
+        <v>5460.056646033359</v>
       </c>
       <c r="AJ18">
-        <v>388.8017955765895</v>
+        <v>388.860401143952</v>
       </c>
       <c r="AK18">
         <v>123.3613359106175</v>
@@ -3735,7 +3735,7 @@
         <v>554.6929574085671</v>
       </c>
       <c r="AN18">
-        <v>1450.344180856995</v>
+        <v>1487.713924862433</v>
       </c>
       <c r="AO18">
         <v>0</v>
@@ -3744,7 +3744,7 @@
         <v>0</v>
       </c>
       <c r="AQ18">
-        <v>1664.571731061642</v>
+        <v>1636.583568840412</v>
       </c>
       <c r="AR18">
         <v>1738.287995910195</v>
@@ -3771,7 +3771,7 @@
         <v>186.0704598983283</v>
       </c>
       <c r="AZ18">
-        <v>844.1062152676626</v>
+        <v>882.9402855749795</v>
       </c>
       <c r="BA18">
         <v>44</v>
@@ -3780,7 +3780,7 @@
         <v>0</v>
       </c>
       <c r="BC18">
-        <v>189.4844433147406</v>
+        <v>228.3185136220575</v>
       </c>
       <c r="BD18">
         <v>548.6821276341473</v>
@@ -3792,10 +3792,10 @@
         <v>1456.184604429749</v>
       </c>
       <c r="BG18">
-        <v>2025.581901198547</v>
+        <v>2026.797771152849</v>
       </c>
       <c r="BH18">
-        <v>97.63410645908858</v>
+        <v>97.69271202645102</v>
       </c>
       <c r="BI18">
         <v>0.6110859106172505</v>
@@ -3806,10 +3806,10 @@
         <v>44651</v>
       </c>
       <c r="B19">
-        <v>-2.339571895058551</v>
+        <v>-7.398079846028857</v>
       </c>
       <c r="C19">
-        <v>-2.848556215275973</v>
+        <v>-2.97895427169459</v>
       </c>
       <c r="E19">
         <v>23157.62470023502</v>
@@ -3830,7 +3830,7 @@
         <v>0.003938803826607495</v>
       </c>
       <c r="K19">
-        <v>1544.279991543916</v>
+        <v>1574.879991543916</v>
       </c>
       <c r="L19">
         <v>756.250632039193</v>
@@ -3842,7 +3842,7 @@
         <v>549.1162193786943</v>
       </c>
       <c r="O19">
-        <v>306.2408068497152</v>
+        <v>306.2938785049959</v>
       </c>
       <c r="P19">
         <v>76.68954672196401</v>
@@ -3881,16 +3881,16 @@
         <v>772.3768478521977</v>
       </c>
       <c r="AB19">
-        <v>1715.334753885363</v>
+        <v>1753.631582933507</v>
       </c>
       <c r="AC19">
         <v>44</v>
       </c>
       <c r="AD19">
-        <v>3480.314439027214</v>
+        <v>3490.923532880751</v>
       </c>
       <c r="AE19">
-        <v>1872.212077636118</v>
+        <v>1882.821171489655</v>
       </c>
       <c r="AF19">
         <v>2313.969670840344</v>
@@ -3917,7 +3917,7 @@
         <v>549.1162193786943</v>
       </c>
       <c r="AN19">
-        <v>1486.324957087421</v>
+        <v>1524.621786135565</v>
       </c>
       <c r="AO19">
         <v>0</v>
@@ -3926,7 +3926,7 @@
         <v>0</v>
       </c>
       <c r="AQ19">
-        <v>1681.27278988823</v>
+        <v>1652.659472731377</v>
       </c>
       <c r="AR19">
         <v>1759.813486320566</v>
@@ -3953,7 +3953,7 @@
         <v>229.0097967979425</v>
       </c>
       <c r="AZ19">
-        <v>852.5472774203392</v>
+        <v>891.7696884307293</v>
       </c>
       <c r="BA19">
         <v>44</v>
@@ -3962,7 +3962,7 @@
         <v>0</v>
       </c>
       <c r="BC19">
-        <v>190.9392877478879</v>
+        <v>230.1616987582779</v>
       </c>
       <c r="BD19">
         <v>554.1561845197784</v>
@@ -3988,10 +3988,10 @@
         <v>44742</v>
       </c>
       <c r="B20">
-        <v>-2.13930466170003</v>
+        <v>-2.312473296450245</v>
       </c>
       <c r="C20">
-        <v>-2.865953568885793</v>
+        <v>-2.18004429017147</v>
       </c>
       <c r="E20">
         <v>23384.06080548141</v>
@@ -4012,7 +4012,7 @@
         <v>0.004387388405960646</v>
       </c>
       <c r="K20">
-        <v>1557.72908484966</v>
+        <v>1588.32908484966</v>
       </c>
       <c r="L20">
         <v>762.8367986466193</v>
@@ -4024,7 +4024,7 @@
         <v>543.5394813488216</v>
       </c>
       <c r="O20">
-        <v>307.9585717819477</v>
+        <v>308.01210563686</v>
       </c>
       <c r="P20">
         <v>77.35743394130677</v>
@@ -4063,16 +4063,16 @@
         <v>764.5327099651686</v>
       </c>
       <c r="AB20">
-        <v>1751.315530115789</v>
+        <v>1790.539444206639</v>
       </c>
       <c r="AC20">
         <v>44</v>
       </c>
       <c r="AD20">
-        <v>3528.521225407126</v>
+        <v>3539.116350869613</v>
       </c>
       <c r="AE20">
-        <v>1911.574510991387</v>
+        <v>1922.169636453873</v>
       </c>
       <c r="AF20">
         <v>2340.913720785433</v>
@@ -4099,7 +4099,7 @@
         <v>543.5394813488216</v>
       </c>
       <c r="AN20">
-        <v>1522.305733317846</v>
+        <v>1561.529647408696</v>
       </c>
       <c r="AO20">
         <v>0</v>
@@ -4108,7 +4108,7 @@
         <v>0</v>
       </c>
       <c r="AQ20">
-        <v>1680.56445339942</v>
+        <v>1651.524008138567</v>
       </c>
       <c r="AR20">
         <v>1781.338976730937</v>
@@ -4135,7 +4135,7 @@
         <v>229.0097967979425</v>
       </c>
       <c r="AZ20">
-        <v>861.5278112361167</v>
+        <v>901.1633819594565</v>
       </c>
       <c r="BA20">
         <v>44</v>
@@ -4144,7 +4144,7 @@
         <v>0</v>
       </c>
       <c r="BC20">
-        <v>231.0100575919666</v>
+        <v>270.6456283153065</v>
       </c>
       <c r="BD20">
         <v>559.5747440544956</v>
@@ -4170,10 +4170,10 @@
         <v>44834</v>
       </c>
       <c r="B21">
-        <v>-0.7357084438719351</v>
+        <v>1.409551007941173</v>
       </c>
       <c r="C21">
-        <v>-1.875296652868696</v>
+        <v>-2.3398235692959</v>
       </c>
       <c r="E21">
         <v>23620.8277944867</v>
@@ -4206,7 +4206,7 @@
         <v>537.9627433189488</v>
       </c>
       <c r="O21">
-        <v>309.8668012505129</v>
+        <v>309.9208485534183</v>
       </c>
       <c r="P21">
         <v>78.09937601365499</v>
@@ -4245,16 +4245,16 @@
         <v>756.6885720781395</v>
       </c>
       <c r="AB21">
-        <v>1784.946656161011</v>
+        <v>1825.097655294567</v>
       </c>
       <c r="AC21">
         <v>44</v>
       </c>
       <c r="AD21">
-        <v>3550.658510453061</v>
+        <v>3561.473045106598</v>
       </c>
       <c r="AE21">
-        <v>1924.717013936188</v>
+        <v>1935.531548589725</v>
       </c>
       <c r="AF21">
         <v>2368.104986202774</v>
@@ -4281,7 +4281,7 @@
         <v>537.9627433189488</v>
       </c>
       <c r="AN21">
-        <v>1558.286509548272</v>
+        <v>1598.437508681828</v>
       </c>
       <c r="AO21">
         <v>0</v>
@@ -4290,7 +4290,7 @@
         <v>0</v>
       </c>
       <c r="AQ21">
-        <v>1655.749688813779</v>
+        <v>1626.556319089618</v>
       </c>
       <c r="AR21">
         <v>1802.864467141307</v>
@@ -4317,7 +4317,7 @@
         <v>226.6601466127393</v>
       </c>
       <c r="AZ21">
-        <v>869.6209405246435</v>
+        <v>909.6288449023414</v>
       </c>
       <c r="BA21">
         <v>44</v>
@@ -4326,7 +4326,7 @@
         <v>0</v>
       </c>
       <c r="BC21">
-        <v>268.9673251224091</v>
+        <v>308.9752295001069</v>
       </c>
       <c r="BD21">
         <v>565.2405190614668</v>

</xml_diff>